<commit_message>
update video and img
</commit_message>
<xml_diff>
--- a/public/botany.xlsx
+++ b/public/botany.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11832" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11832"/>
   </bookViews>
   <sheets>
     <sheet name="Botany" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="382">
   <si>
     <t>Botany Branch</t>
   </si>
@@ -1075,9 +1075,6 @@
     <t>প্রাণীজগৎ পরিচিতি</t>
   </si>
   <si>
-    <t>প্রাণীজগৎ হলো জীবজগতের একটি প্রধান অংশ, যেখানে বিভিন্ন প্রজাতির প্রাণী অন্তর্ভুক্ত হয়। এদের রয়েছে কোষীয় গঠন, সচলতা ও চেতনা।</t>
-  </si>
-  <si>
     <t>শ্রেণিবিন্যাসের উদ্দেশ্য</t>
   </si>
   <si>
@@ -1141,9 +1138,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>কোষতত্ত্ব হলো একটি জীববৈজ্ঞানিক তত্ত্ব যা বলে যে সকল জীব কোষ দ্বারা গঠিত এবং কোষ জীবনের গঠন ও কার্যকারণের মৌলিক একক। ৷ উদাহরণ : মানবদেহ, গাছ, ব্যাকটেরিয়া সবই কোষ দিয়ে গঠিত। (test data)</t>
-  </si>
-  <si>
     <t>/images/plant1.jpg</t>
   </si>
   <si>
@@ -1163,6 +1157,22 @@
   </si>
   <si>
     <t>/video/video1.mp4</t>
+  </si>
+  <si>
+    <t>প্রাণীজগৎ হলো জীবজগতের একটি প্রধান অংশ, যেখানে বিভিন্ন প্রজাতির প্রাণী অন্তর্ভুক্ত হয়। এদের রয়েছে কোষীয় গঠন, সচলতা ও চেতনা।
+প্রাণীজগৎ হলো জীবজগতের একটি প্রধান অংশ, যেখানে বিভিন্ন প্রজাতির প্রাণী অন্তর্ভুক্ত হয়। এদের রয়েছে কোষীয় গঠন, সচলতা ও চেতনা।
+প্রাণীজগৎ হলো জীবজগতের একটি প্রধান অংশ, যেখানে বিভিন্ন প্রজাতির প্রাণী অন্তর্ভুক্ত হয়। এদের রয়েছে কোষীয় গঠন, সচলতা ও চেতনা।
+Cell theory is a biological theory that states all living organisms are made up of cells, and the cell is the basic unit of structure and function in living beings.
+Example: The human body, plants, and bacteria are all made up of cells.
+Cell theory is a biological theory that states all living organisms are made up of cells, and the cell is the basic unit of structure and function in living beings.
+Example: The human body, plants, and bacteria are all made up of cells.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">কোষতত্ত্ব হলো একটি জীববৈজ্ঞানিক তত্ত্ব যা বলে যে সকল জীব কোষ দ্বারা গঠিত এবং কোষ জীবনের গঠন ও কার্যকারণের মৌলিক একক। ৷ উদাহরণ : মানবদেহ, গাছ, ব্যাকটেরিয়া সবই কোষ দিয়ে গঠিত।
+Plant cells are eukaryotic cells forming the building blocks of plants, characterized by a cell wall for rigidity, a large central vacuole for turgor pressure and storage, and chloroplasts for photosynthesis. These unique organelles, along with a nucleus, cell membrane, and cytoplasm, enable plant cells to maintain structure, store nutrients, and produce energy through photosynthesis, making them distinctly different from animal cells. </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7ybxaYhRpIA</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1325,6 +1335,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1546,8 +1559,8 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1557,6 +1570,7 @@
     <col min="3" max="3" width="29.109375" customWidth="1"/>
     <col min="4" max="4" width="72.44140625" customWidth="1"/>
     <col min="5" max="5" width="63.6640625" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" customWidth="1"/>
     <col min="7" max="7" width="12.88671875" customWidth="1"/>
     <col min="8" max="8" width="20.88671875" customWidth="1"/>
     <col min="10" max="10" width="36.44140625" customWidth="1"/>
@@ -1576,10 +1590,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1590,10 +1607,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>374</v>
+        <v>372</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>378</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1613,7 +1633,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
@@ -1628,6 +1651,9 @@
       </c>
       <c r="D4" s="6" t="s">
         <v>11</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
@@ -8062,6 +8088,10 @@
       <c r="D1000" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8070,8 +8100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8098,13 +8128,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>348</v>
       </c>
@@ -8114,14 +8144,14 @@
       <c r="C2" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>351</v>
+      <c r="D2" s="18" t="s">
+        <v>379</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8132,17 +8162,15 @@
         <v>349</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>353</v>
-      </c>
       <c r="E3" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>380</v>
-      </c>
+        <v>375</v>
+      </c>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -8152,10 +8180,10 @@
         <v>349</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>354</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8166,10 +8194,10 @@
         <v>349</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8180,10 +8208,10 @@
         <v>349</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8194,10 +8222,10 @@
         <v>349</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8208,10 +8236,10 @@
         <v>349</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8222,10 +8250,10 @@
         <v>349</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8236,10 +8264,10 @@
         <v>349</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -8250,10 +8278,10 @@
         <v>349</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8264,10 +8292,10 @@
         <v>349</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -8278,10 +8306,10 @@
         <v>349</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8292,10 +8320,10 @@
         <v>349</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -8306,10 +8334,10 @@
         <v>349</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8320,10 +8348,10 @@
         <v>349</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -8334,10 +8362,10 @@
         <v>349</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -8348,10 +8376,10 @@
         <v>349</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -8362,10 +8390,10 @@
         <v>349</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -8376,10 +8404,10 @@
         <v>349</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -8390,290 +8418,290 @@
         <v>349</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>359</v>
-      </c>
       <c r="C22" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>361</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D23" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D24" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D25" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D26" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D27" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D28" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D29" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D30" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D31" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D32" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D33" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D34" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D35" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D36" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="C37" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D37" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="C38" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D38" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D39" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="C40" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D40" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="D41" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>